<commit_message>
Update API with new GlobalSchema version, which includes Project_V2 ECClass         -Update pyCApiGen tool to handle dateTime property types                 -Run tool to generate updated Api         -Update integration tests with new properties                 -Change ASSERTs to EXPECTs when WSG instance is created, to ensure it is deleted on failure
</commit_message>
<xml_diff>
--- a/iModelBridgeCore/WSClient/ConnectC/Tools/pyCApiGen/autoGenClasses.xlsx
+++ b/iModelBridgeCore/WSClient/ConnectC/Tools/pyCApiGen/autoGenClasses.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="29">
   <si>
     <t>ECClass Name - must be exactly specified per ECSchema</t>
   </si>
@@ -69,24 +69,6 @@
     <t>ProjectProperties</t>
   </si>
   <si>
-    <t>ProjectTemplate</t>
-  </si>
-  <si>
-    <t>Organization_SQLAzure_PoC</t>
-  </si>
-  <si>
-    <t>Project_SQLAzure_PoC</t>
-  </si>
-  <si>
-    <t>ProjectFavorite_SQLAzure_PoC</t>
-  </si>
-  <si>
-    <t>ProjectMRU_SQLAzure_Poc</t>
-  </si>
-  <si>
-    <t>ProjectMRUDetail_SQLAzure_PoC</t>
-  </si>
-  <si>
     <t>NOTE: If all C,R,U,D,ReadAll columns are red (FALSE) for a given row, the corresponding ECClass will be excluded from the API</t>
   </si>
   <si>
@@ -112,6 +94,18 @@
   </si>
   <si>
     <t>BentleyCONNECT.Global--CONNECT.GLOBAL</t>
+  </si>
+  <si>
+    <t>Project_V2</t>
+  </si>
+  <si>
+    <t>ProjectFavorite_V2</t>
+  </si>
+  <si>
+    <t>ProjectMRUDetail_V2</t>
+  </si>
+  <si>
+    <t>ProjectProperties_V2</t>
   </si>
 </sst>
 </file>
@@ -307,6 +301,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -316,21 +319,502 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="120">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -958,10 +1442,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:W29"/>
+  <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -977,31 +1461,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="34.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="14"/>
+      <c r="A1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:23" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>26</v>
+        <v>18</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>0</v>
@@ -1021,34 +1505,34 @@
       <c r="J2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>7</v>
@@ -1072,16 +1556,16 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>8</v>
@@ -1105,16 +1589,16 @@
     </row>
     <row r="5" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>9</v>
@@ -1138,30 +1622,30 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="F6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="2" t="b">
         <v>1</v>
@@ -1170,27 +1654,27 @@
         <v>1</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="2" t="b">
         <v>1</v>
@@ -1199,28 +1683,30 @@
         <v>0</v>
       </c>
       <c r="I7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="K7" s="6"/>
+      <c r="K7" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F8" s="2" t="b">
         <v>0</v>
@@ -1232,7 +1718,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="2" t="b">
         <v>1</v>
@@ -1243,25 +1729,25 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="2" t="b">
         <v>0</v>
@@ -1269,32 +1755,32 @@
       <c r="I9" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J9" s="1" t="b">
-        <v>0</v>
+      <c r="J9" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="G10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="2" t="b">
         <v>0</v>
@@ -1302,32 +1788,34 @@
       <c r="I10" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J10" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K10" s="6"/>
+      <c r="J10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="G11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="2" t="b">
         <v>0</v>
@@ -1335,26 +1823,28 @@
       <c r="I11" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J11" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" s="6"/>
+      <c r="J11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F12" s="2" t="b">
         <v>0</v>
@@ -1375,19 +1865,19 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>19</v>
       </c>
       <c r="F13" s="2" t="b">
         <v>0</v>
@@ -1406,284 +1896,250 @@
       </c>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="28" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="L2:W2"/>
     <mergeCell ref="A1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="F8:I15">
-    <cfRule type="containsText" dxfId="49" priority="55" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="F10:I10 F12:I12">
+    <cfRule type="containsText" dxfId="93" priority="75" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="92" priority="76" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:I4">
+    <cfRule type="containsText" dxfId="91" priority="65" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="90" priority="66" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3">
+    <cfRule type="containsText" dxfId="89" priority="69" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="88" priority="70" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="containsText" dxfId="87" priority="67" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",I3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="86" priority="68" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",I3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9:I9">
+    <cfRule type="containsText" dxfId="85" priority="63" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="84" priority="64" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:I6">
+    <cfRule type="containsText" dxfId="83" priority="61" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="82" priority="62" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7">
+    <cfRule type="containsText" dxfId="81" priority="59" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",G7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="80" priority="60" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",G7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="containsText" dxfId="79" priority="55" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",I7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="78" priority="56" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",I7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7">
+    <cfRule type="containsText" dxfId="77" priority="53" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="76" priority="54" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
+    <cfRule type="containsText" dxfId="75" priority="51" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="74" priority="52" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="containsText" dxfId="73" priority="49" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",G3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="72" priority="50" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",G3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3">
+    <cfRule type="containsText" dxfId="71" priority="47" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="48" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:K3">
+    <cfRule type="containsText" dxfId="69" priority="45" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="68" priority="46" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J12:K12">
+    <cfRule type="containsText" dxfId="67" priority="43" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="66" priority="44" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:K9">
+    <cfRule type="containsText" dxfId="63" priority="27" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="28" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7:K7">
+    <cfRule type="containsText" dxfId="61" priority="25" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="60" priority="26" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:K5 K6">
+    <cfRule type="containsText" dxfId="59" priority="23" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="24" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4:K4">
+    <cfRule type="containsText" dxfId="57" priority="21" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="56" priority="22" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:K10">
+    <cfRule type="containsText" dxfId="55" priority="29" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="30" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6">
+    <cfRule type="containsText" dxfId="53" priority="19" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="20" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="containsText" dxfId="45" priority="17" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",G8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="18" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",G8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
+    <cfRule type="containsText" dxfId="43" priority="15" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",I8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="16" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",I8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8:K8">
+    <cfRule type="containsText" dxfId="41" priority="9" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="10" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11:K11">
+    <cfRule type="containsText" dxfId="39" priority="5" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="6" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="56" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:I4">
-    <cfRule type="containsText" dxfId="47" priority="45" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="46" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3">
-    <cfRule type="containsText" dxfId="45" priority="49" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="50" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
-    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",I3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="48" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",I3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F7:I7">
-    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5:I5">
-    <cfRule type="containsText" dxfId="39" priority="41" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="42" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",G6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="40" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",G6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
-    <cfRule type="containsText" dxfId="35" priority="35" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",I6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="36" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",I6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6">
-    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6">
-    <cfRule type="containsText" dxfId="31" priority="31" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3">
-    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",G3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",G3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3">
-    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3:K3">
-    <cfRule type="containsText" dxfId="25" priority="25" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9:K9">
-    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10:K10">
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J11:K11">
-    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J12:K12">
-    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J12)))</formula>
+  <conditionalFormatting sqref="H8">
+    <cfRule type="containsText" dxfId="15" priority="11" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11:I11">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13:I13">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13:K13">
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J14:K14">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J15:K15">
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J8:K8">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J7:K7">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J6:K6">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J5:K5">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J4:K4">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Please enter TRUE or FALSE" error="Only &quot;TRUE&quot;, or &quot;FALSE&quot; are allowed values. Please enter a valid value." sqref="F5 F7 F3:J3 J9:J15">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Please enter TRUE or FALSE" error="Only &quot;TRUE&quot;, or &quot;FALSE&quot; are allowed values. Please enter a valid value." sqref="J12:J13 F9 F3:J3 F5:F6 G6:J6">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Enter a valid CRUD function" error="Only &quot;Create&quot;, &quot;Read&quot;, &quot;Update&quot;, or &quot;Delete&quot; are allowed values. Please enter a valid value." sqref="F4 F6 F8:F15 G4:I15 J4:J8">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Enter a valid CRUD function" error="Only &quot;Create&quot;, &quot;Read&quot;, &quot;Update&quot;, or &quot;Delete&quot; are allowed values. Please enter a valid value." sqref="F4 J8:J11 F7:F8 G4:J5 G7:J7 F10:F13 G8:I13">
       <formula1>"True, False"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update CC Wrapper with new schema SRB: Daniel.Delaney
</commit_message>
<xml_diff>
--- a/iModelBridgeCore/WSClient/ConnectC/Tools/pyCApiGen/autoGenClasses.xlsx
+++ b/iModelBridgeCore/WSClient/ConnectC/Tools/pyCApiGen/autoGenClasses.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\dgndb0601dev\src\WSClient\ConnectC\Tools\pyCApiGen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bim0200\src\WSClient\ConnectC\Tools\pyCApiGen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="40">
   <si>
     <t>ECClass Name - must be exactly specified per ECSchema</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Schema filename</t>
   </si>
   <si>
-    <t>N~3AGlobalSchema.01.00.xml</t>
-  </si>
-  <si>
     <t>RepositoryId</t>
   </si>
   <si>
@@ -106,12 +103,48 @@
   </si>
   <si>
     <t>ProjectProperties_V2</t>
+  </si>
+  <si>
+    <t>Organization_V2</t>
+  </si>
+  <si>
+    <t>Project_V3</t>
+  </si>
+  <si>
+    <t>Project_V4</t>
+  </si>
+  <si>
+    <t>ProjectFavorite_V3</t>
+  </si>
+  <si>
+    <t>ProjectFavorite_V4</t>
+  </si>
+  <si>
+    <t>ProjectMRUDetail_V3</t>
+  </si>
+  <si>
+    <t>ProjectMRUDetail_V4</t>
+  </si>
+  <si>
+    <t>OrgProject</t>
+  </si>
+  <si>
+    <t>ProjectProperties_V3</t>
+  </si>
+  <si>
+    <t>eBBacked,LinkToAssetType,LinkToIndustry, LinkToIndustryAssets, PWDMInvitationId, IsRbacEnabled</t>
+  </si>
+  <si>
+    <t>PWDMInvitationId, IsRbacEnabled</t>
+  </si>
+  <si>
+    <t>Schema_12_13_2016.xml</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -324,175 +357,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
-  <dxfs count="120">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="96">
     <dxf>
       <fill>
         <patternFill>
@@ -1442,16 +1307,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:W26"/>
+  <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.77734375" customWidth="1"/>
-    <col min="2" max="3" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="41.5546875" customWidth="1"/>
     <col min="4" max="4" width="18.109375" customWidth="1"/>
     <col min="5" max="5" width="29.88671875" style="7" customWidth="1"/>
     <col min="6" max="6" width="7.6640625" style="7" customWidth="1"/>
@@ -1479,7 +1345,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>21</v>
@@ -1526,10 +1392,10 @@
         <v>19</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>17</v>
@@ -1559,10 +1425,10 @@
         <v>19</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>17</v>
@@ -1571,10 +1437,10 @@
         <v>8</v>
       </c>
       <c r="F4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="2" t="b">
         <v>0</v>
@@ -1583,25 +1449,25 @@
         <v>0</v>
       </c>
       <c r="J4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="F5" s="2" t="b">
         <v>1</v>
@@ -1610,33 +1476,31 @@
         <v>1</v>
       </c>
       <c r="H5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="K5" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F6" s="2" t="b">
         <v>1</v>
@@ -1653,101 +1517,99 @@
       <c r="J6" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="K6" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F7" s="2" t="b">
         <v>0</v>
       </c>
       <c r="G7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="2" t="b">
         <v>0</v>
       </c>
       <c r="I7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F8" s="2" t="b">
         <v>0</v>
       </c>
       <c r="G8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="2" t="b">
         <v>0</v>
       </c>
       <c r="I8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="2" t="b">
         <v>0</v>
@@ -1756,66 +1618,68 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K9" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="F10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="2" t="b">
         <v>1</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="G11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="2" t="b">
         <v>0</v>
@@ -1824,7 +1688,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="6" t="s">
         <v>12</v>
@@ -1835,16 +1699,16 @@
         <v>19</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F12" s="2" t="b">
         <v>0</v>
@@ -1858,26 +1722,28 @@
       <c r="I12" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J12" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K12" s="6"/>
+      <c r="J12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F13" s="2" t="b">
         <v>0</v>
@@ -1891,255 +1757,716 @@
       <c r="I13" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J13" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" s="6"/>
+      <c r="J13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="25" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" s="6"/>
+    </row>
+    <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="L2:W2"/>
     <mergeCell ref="A1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="F10:I10 F12:I12">
-    <cfRule type="containsText" dxfId="93" priority="75" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="76" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F10)))</formula>
+  <conditionalFormatting sqref="F16:I16 F20:I20 G17:G18">
+    <cfRule type="containsText" dxfId="95" priority="127" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="94" priority="128" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6:I6 H7:I9">
+    <cfRule type="containsText" dxfId="93" priority="117" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="92" priority="118" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3">
+    <cfRule type="containsText" dxfId="91" priority="121" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="90" priority="122" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="containsText" dxfId="89" priority="119" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",I3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="88" priority="120" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",I3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15:I15">
+    <cfRule type="containsText" dxfId="87" priority="115" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="86" priority="116" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7:G7 F10:I10 F8:F9">
+    <cfRule type="containsText" dxfId="85" priority="113" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="84" priority="114" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:G13">
+    <cfRule type="containsText" dxfId="83" priority="111" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",G11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="82" priority="112" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",G11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11:I13">
+    <cfRule type="containsText" dxfId="81" priority="107" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",I11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="80" priority="108" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",I11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="containsText" dxfId="79" priority="105" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="78" priority="106" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="containsText" dxfId="77" priority="103" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="76" priority="104" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="containsText" dxfId="75" priority="101" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",G3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="74" priority="102" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",G3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3">
+    <cfRule type="containsText" dxfId="73" priority="99" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="72" priority="100" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:K3">
+    <cfRule type="containsText" dxfId="71" priority="97" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="98" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J20:K20">
+    <cfRule type="containsText" dxfId="69" priority="95" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="68" priority="96" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15:K15">
+    <cfRule type="containsText" dxfId="67" priority="79" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="66" priority="80" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11:K11 J12:J13">
+    <cfRule type="containsText" dxfId="65" priority="77" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="78" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7:K7 K10 J8:J9">
+    <cfRule type="containsText" dxfId="63" priority="75" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="76" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6:K6">
+    <cfRule type="containsText" dxfId="61" priority="73" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="60" priority="74" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16:K16 J17:J18">
+    <cfRule type="containsText" dxfId="59" priority="81" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="82" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10">
+    <cfRule type="containsText" dxfId="57" priority="71" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="56" priority="72" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14">
+    <cfRule type="containsText" dxfId="55" priority="69" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",G14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="70" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",G14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14">
+    <cfRule type="containsText" dxfId="53" priority="67" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",I14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="68" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",I14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J14:K14">
+    <cfRule type="containsText" dxfId="51" priority="61" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="62" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J19:K19">
+    <cfRule type="containsText" dxfId="49" priority="57" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="58" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14">
+    <cfRule type="containsText" dxfId="47" priority="65" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="66" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14">
+    <cfRule type="containsText" dxfId="45" priority="63" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="64" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19:I19">
+    <cfRule type="containsText" dxfId="43" priority="59" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="60" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22:I22">
+    <cfRule type="containsText" dxfId="41" priority="55" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="56" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J22:K22">
+    <cfRule type="containsText" dxfId="39" priority="53" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="54" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:I4">
-    <cfRule type="containsText" dxfId="91" priority="65" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="37" priority="51" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="66" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="36" priority="52" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3">
-    <cfRule type="containsText" dxfId="89" priority="69" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="70" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
-    <cfRule type="containsText" dxfId="87" priority="67" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",I3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="68" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",I3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F9:I9">
-    <cfRule type="containsText" dxfId="85" priority="63" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="64" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5:I6">
-    <cfRule type="containsText" dxfId="83" priority="61" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="J4:K4">
+    <cfRule type="containsText" dxfId="35" priority="49" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="50" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8:G9">
+    <cfRule type="containsText" dxfId="33" priority="47" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",G8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="48" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",G8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8">
+    <cfRule type="containsText" dxfId="31" priority="45" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="46" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12">
+    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12">
+    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="containsText" dxfId="25" priority="39" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="40" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K12">
+    <cfRule type="containsText" dxfId="23" priority="27" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="28" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
+    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="containsText" dxfId="17" priority="21" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="22" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18 H18:I18">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17 H17:I17">
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J21:K21">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21:I21">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:I5">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="62" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
-    <cfRule type="containsText" dxfId="81" priority="59" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",G7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="60" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",G7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
-    <cfRule type="containsText" dxfId="79" priority="55" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",I7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="56" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",I7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F7">
-    <cfRule type="containsText" dxfId="77" priority="53" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="54" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
-    <cfRule type="containsText" dxfId="75" priority="51" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="52" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3">
-    <cfRule type="containsText" dxfId="73" priority="49" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",G3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="50" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",G3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3">
-    <cfRule type="containsText" dxfId="71" priority="47" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="48" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3:K3">
-    <cfRule type="containsText" dxfId="69" priority="45" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="46" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J12:K12">
-    <cfRule type="containsText" dxfId="67" priority="43" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="44" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9:K9">
-    <cfRule type="containsText" dxfId="63" priority="27" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="28" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J7:K7">
-    <cfRule type="containsText" dxfId="61" priority="25" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="26" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J5:K5 K6">
-    <cfRule type="containsText" dxfId="59" priority="23" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="J5:K5">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="24" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J4:K4">
-    <cfRule type="containsText" dxfId="57" priority="21" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="22" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10:K10">
-    <cfRule type="containsText" dxfId="55" priority="29" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="30" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J6">
-    <cfRule type="containsText" dxfId="53" priority="19" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="20" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
-    <cfRule type="containsText" dxfId="45" priority="17" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",G8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="18" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",G8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
-    <cfRule type="containsText" dxfId="43" priority="15" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",I8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="16" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",I8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J8:K8">
-    <cfRule type="containsText" dxfId="41" priority="9" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="10" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J11:K11">
-    <cfRule type="containsText" dxfId="39" priority="5" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="6" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
-    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
-    <cfRule type="containsText" dxfId="15" priority="11" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F11:I11">
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F13:I13">
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J13:K13">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Please enter TRUE or FALSE" error="Only &quot;TRUE&quot;, or &quot;FALSE&quot; are allowed values. Please enter a valid value." sqref="J12:J13 F9 F3:J3 F5:F6 G6:J6">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Please enter TRUE or FALSE" error="Only &quot;TRUE&quot;, or &quot;FALSE&quot; are allowed values. Please enter a valid value." sqref="H10:J10 F15 F3:J3 G8:G10 F7:F10 J20:J22">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Enter a valid CRUD function" error="Only &quot;Create&quot;, &quot;Read&quot;, &quot;Update&quot;, or &quot;Delete&quot; are allowed values. Please enter a valid value." sqref="F4 J8:J11 F7:F8 G4:J5 G7:J7 F10:F13 G8:I13">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Enter a valid CRUD function" error="Only &quot;Create&quot;, &quot;Read&quot;, &quot;Update&quot;, or &quot;Delete&quot; are allowed values. Please enter a valid value." sqref="H5:J9 G5:G7 G11:J16 G17:I22 F11:F14 J17:J19 F16:F22 G4:J4 F4:F6">
       <formula1>"True, False"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
ConnectC Schema & Test update.
</commit_message>
<xml_diff>
--- a/iModelBridgeCore/WSClient/ConnectC/Tools/pyCApiGen/autoGenClasses.xlsx
+++ b/iModelBridgeCore/WSClient/ConnectC/Tools/pyCApiGen/autoGenClasses.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bim0200\src\WSClient\ConnectC\Tools\pyCApiGen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\builds\bim0200dev\src\WSClient\ConnectC\Tools\pyCApiGen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="38">
   <si>
     <t>ECClass Name - must be exactly specified per ECSchema</t>
   </si>
@@ -130,12 +130,6 @@
   </si>
   <si>
     <t>ProjectProperties_V3</t>
-  </si>
-  <si>
-    <t>eBBacked,LinkToAssetType,LinkToIndustry, LinkToIndustryAssets, PWDMInvitationId, IsRbacEnabled</t>
-  </si>
-  <si>
-    <t>PWDMInvitationId, IsRbacEnabled</t>
   </si>
   <si>
     <t>Schema_12_13_2016.xml</t>
@@ -1310,7 +1304,7 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1395,7 +1389,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>17</v>
@@ -1428,7 +1422,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>17</v>
@@ -1461,7 +1455,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>17</v>
@@ -1494,7 +1488,7 @@
         <v>23</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>17</v>
@@ -1527,7 +1521,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>17</v>
@@ -1562,7 +1556,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>17</v>
@@ -1597,7 +1591,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>17</v>
@@ -1632,7 +1626,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>17</v>
@@ -1656,7 +1650,7 @@
         <v>1</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1667,7 +1661,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>17</v>
@@ -1702,7 +1696,7 @@
         <v>23</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>17</v>
@@ -1737,7 +1731,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>17</v>
@@ -1772,7 +1766,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>17</v>
@@ -1796,7 +1790,7 @@
         <v>1</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
@@ -1807,7 +1801,7 @@
         <v>23</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>17</v>
@@ -1840,7 +1834,7 @@
         <v>23</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>17</v>
@@ -1875,7 +1869,7 @@
         <v>23</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>17</v>
@@ -1910,7 +1904,7 @@
         <v>23</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>17</v>
@@ -1945,7 +1939,7 @@
         <v>23</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>17</v>
@@ -1969,7 +1963,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1980,7 +1974,7 @@
         <v>23</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>17</v>
@@ -2013,7 +2007,7 @@
         <v>23</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>17</v>
@@ -2046,7 +2040,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Adding Generated Project Share code to CWSCC lib.
</commit_message>
<xml_diff>
--- a/iModelBridgeCore/WSClient/ConnectC/Tools/pyCApiGen/autoGenClasses.xlsx
+++ b/iModelBridgeCore/WSClient/ConnectC/Tools/pyCApiGen/autoGenClasses.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,11 +15,12 @@
     <sheet name="autoGenClasses" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="51">
   <si>
     <t>ECClass Name - must be exactly specified per ECSchema</t>
   </si>
@@ -133,6 +134,45 @@
   </si>
   <si>
     <t>Schema_12_13_2016.xml</t>
+  </si>
+  <si>
+    <t>BentleyCONNECT--Main</t>
+  </si>
+  <si>
+    <t>Schema_ProjectShare_03_16_2017.xml</t>
+  </si>
+  <si>
+    <t>ProjectShare</t>
+  </si>
+  <si>
+    <t>AutomationType</t>
+  </si>
+  <si>
+    <t>DeletePropertyMap</t>
+  </si>
+  <si>
+    <t>DeletePropertyTimeStampMap</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Folder</t>
+  </si>
+  <si>
+    <t>PublishSettings</t>
+  </si>
+  <si>
+    <t>ProjectPermission</t>
+  </si>
+  <si>
+    <t>PublishFile</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>ConnectWsgProjectShare</t>
   </si>
 </sst>
 </file>
@@ -351,7 +391,259 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="132">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1303,14 +1595,14 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.5546875" customWidth="1"/>
     <col min="4" max="4" width="18.109375" customWidth="1"/>
     <col min="5" max="5" width="29.88671875" style="7" customWidth="1"/>
@@ -2065,6 +2357,303 @@
       </c>
       <c r="K22" s="6"/>
     </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" s="6"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K28" s="6"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" s="6"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" s="6"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K31" s="6"/>
+    </row>
     <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
@@ -2073,394 +2662,538 @@
     <mergeCell ref="A1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="F16:I16 F20:I20 G17:G18">
-    <cfRule type="containsText" dxfId="95" priority="127" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="131" priority="167" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="128" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="130" priority="168" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:I6 H7:I9">
-    <cfRule type="containsText" dxfId="93" priority="117" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="129" priority="157" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="118" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="128" priority="158" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="containsText" dxfId="91" priority="121" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="127" priority="161" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="122" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="126" priority="162" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="containsText" dxfId="89" priority="119" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="125" priority="159" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",I3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="120" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="124" priority="160" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",I3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15:I15">
-    <cfRule type="containsText" dxfId="87" priority="115" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="123" priority="155" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="116" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="122" priority="156" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:G7 F10:I10 F8:F9">
-    <cfRule type="containsText" dxfId="85" priority="113" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="121" priority="153" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="114" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="120" priority="154" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:G13">
-    <cfRule type="containsText" dxfId="83" priority="111" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="119" priority="151" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="112" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="118" priority="152" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:I13">
-    <cfRule type="containsText" dxfId="81" priority="107" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="117" priority="147" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",I11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="108" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="116" priority="148" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",I11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="containsText" dxfId="79" priority="105" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="115" priority="145" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="106" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="114" priority="146" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="containsText" dxfId="77" priority="103" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="113" priority="143" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="104" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="112" priority="144" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="containsText" dxfId="75" priority="101" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="111" priority="141" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="102" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="110" priority="142" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="containsText" dxfId="73" priority="99" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="109" priority="139" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="100" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="108" priority="140" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:K3">
-    <cfRule type="containsText" dxfId="71" priority="97" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="107" priority="137" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="98" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="106" priority="138" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:K20">
-    <cfRule type="containsText" dxfId="69" priority="95" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="105" priority="135" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="96" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="104" priority="136" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:K15">
-    <cfRule type="containsText" dxfId="67" priority="79" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="103" priority="119" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="80" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="102" priority="120" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:K11 J12:J13">
-    <cfRule type="containsText" dxfId="65" priority="77" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="101" priority="117" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="78" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="100" priority="118" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:K7 K10 J8:J9">
-    <cfRule type="containsText" dxfId="63" priority="75" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="99" priority="115" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="76" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="98" priority="116" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:K6">
-    <cfRule type="containsText" dxfId="61" priority="73" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="97" priority="113" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="74" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="96" priority="114" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:K16 J17:J18">
-    <cfRule type="containsText" dxfId="59" priority="81" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="95" priority="121" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="82" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="94" priority="122" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="containsText" dxfId="57" priority="71" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="93" priority="111" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="72" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="92" priority="112" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14">
-    <cfRule type="containsText" dxfId="55" priority="69" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="91" priority="109" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="70" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="90" priority="110" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="containsText" dxfId="53" priority="67" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="89" priority="107" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",I14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="68" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="88" priority="108" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",I14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:K14">
-    <cfRule type="containsText" dxfId="51" priority="61" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="87" priority="101" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="62" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="86" priority="102" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:K19">
-    <cfRule type="containsText" dxfId="49" priority="57" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="85" priority="97" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="58" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="84" priority="98" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="containsText" dxfId="47" priority="65" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="83" priority="105" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="66" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="82" priority="106" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="containsText" dxfId="45" priority="63" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="81" priority="103" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="64" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="80" priority="104" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19:I19">
-    <cfRule type="containsText" dxfId="43" priority="59" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="79" priority="99" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="60" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="78" priority="100" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22:I22">
-    <cfRule type="containsText" dxfId="41" priority="55" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="77" priority="95" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="56" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="76" priority="96" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:K22">
-    <cfRule type="containsText" dxfId="39" priority="53" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="75" priority="93" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="54" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="74" priority="94" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:I4">
-    <cfRule type="containsText" dxfId="37" priority="51" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="73" priority="91" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="52" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="72" priority="92" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:K4">
-    <cfRule type="containsText" dxfId="35" priority="49" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="71" priority="89" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="50" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="70" priority="90" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G9">
-    <cfRule type="containsText" dxfId="33" priority="47" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="69" priority="87" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="48" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="68" priority="88" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="containsText" dxfId="31" priority="45" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="67" priority="85" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",K8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="46" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="66" priority="86" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",K8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="65" priority="69" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="64" priority="70" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
+    <cfRule type="containsText" dxfId="63" priority="71" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="72" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="containsText" dxfId="61" priority="79" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="60" priority="80" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K12">
+    <cfRule type="containsText" dxfId="59" priority="67" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="68" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
+    <cfRule type="containsText" dxfId="57" priority="59" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="56" priority="60" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13">
+    <cfRule type="containsText" dxfId="55" priority="57" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="58" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="containsText" dxfId="53" priority="61" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="62" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18 H18:I18">
+    <cfRule type="containsText" dxfId="51" priority="55" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="56" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="containsText" dxfId="49" priority="53" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="54" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="containsText" dxfId="47" priority="49" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="50" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17 H17:I17">
+    <cfRule type="containsText" dxfId="45" priority="51" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="52" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J21:K21">
+    <cfRule type="containsText" dxfId="43" priority="45" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="46" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21:I21">
+    <cfRule type="containsText" dxfId="41" priority="47" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="48" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:I5">
+    <cfRule type="containsText" dxfId="39" priority="43" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="44" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:K5">
+    <cfRule type="containsText" dxfId="37" priority="41" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="42" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F23:I23">
+    <cfRule type="containsText" dxfId="35" priority="39" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="40" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J23:K23">
+    <cfRule type="containsText" dxfId="33" priority="37" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="38" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24:I24">
+    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J24:K24">
+    <cfRule type="containsText" dxfId="29" priority="33" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="34" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25:I25">
     <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F12)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F25)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="containsText" dxfId="25" priority="39" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",K9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="40" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",K9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K12">
-    <cfRule type="containsText" dxfId="23" priority="27" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",K12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="28" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",K12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
-    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",H13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",H13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K13">
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",K13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",K13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F13">
-    <cfRule type="containsText" dxfId="17" priority="21" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="22" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F18 H18:I18">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J25:K25">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26:I26">
+    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J26:K26">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27:I27">
+    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J27:K27">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F28:I28">
     <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F28)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J28:K28">
     <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",K18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",J28)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",K18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K17">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",K17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",K17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F17 H17:I17">
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J21:K21">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F21:I21">
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5:I5">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F29:I29">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J29:K29">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F30:I30">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J30:K30">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F31:I31">
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F5)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F31)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J5:K5">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J31:K31">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",J5)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",J31)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",J5)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",J31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Please enter TRUE or FALSE" error="Only &quot;TRUE&quot;, or &quot;FALSE&quot; are allowed values. Please enter a valid value." sqref="H10:J10 F15 F3:J3 G8:G10 F7:F10 J20:J22">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Please enter TRUE or FALSE" error="Only &quot;TRUE&quot;, or &quot;FALSE&quot; are allowed values. Please enter a valid value." sqref="H10:J10 F15 F3:J3 G8:G10 F7:F10 J20:J31">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Enter a valid CRUD function" error="Only &quot;Create&quot;, &quot;Read&quot;, &quot;Update&quot;, or &quot;Delete&quot; are allowed values. Please enter a valid value." sqref="H5:J9 G5:G7 G11:J16 G17:I22 F11:F14 J17:J19 F16:F22 G4:J4 F4:F6">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Enter a valid CRUD function" error="Only &quot;Create&quot;, &quot;Read&quot;, &quot;Update&quot;, or &quot;Delete&quot; are allowed values. Please enter a valid value." sqref="H5:J9 G5:G7 G11:J16 F16:F31 F11:F14 J17:J19 F4:F6 G4:J4 G17:I31">
       <formula1>"True, False"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
WIP: Adding code gen for structs and init and free methods for ECRelationShipClass elements in a schema doc.
</commit_message>
<xml_diff>
--- a/iModelBridgeCore/WSClient/ConnectC/Tools/pyCApiGen/autoGenClasses.xlsx
+++ b/iModelBridgeCore/WSClient/ConnectC/Tools/pyCApiGen/autoGenClasses.xlsx
@@ -9,18 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="3624"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12270" windowHeight="3630" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="autoGenClasses" sheetId="1" r:id="rId1"/>
+    <sheet name="Relationships" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="59">
   <si>
     <t>ECClass Name - must be exactly specified per ECSchema</t>
   </si>
@@ -173,6 +173,30 @@
   </si>
   <si>
     <t>ConnectWsgProjectShare</t>
+  </si>
+  <si>
+    <t>Specify relationships and function onto which the relationship should be applied</t>
+  </si>
+  <si>
+    <t>On Create</t>
+  </si>
+  <si>
+    <t>On Read</t>
+  </si>
+  <si>
+    <t>On Update</t>
+  </si>
+  <si>
+    <t>On Delete</t>
+  </si>
+  <si>
+    <t>On ReadAll</t>
+  </si>
+  <si>
+    <t>ECRelationshpClass Name - must be exactly specified per ECSchema</t>
+  </si>
+  <si>
+    <t>FolderHasContent</t>
   </si>
 </sst>
 </file>
@@ -391,7 +415,133 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
-  <dxfs count="132">
+  <dxfs count="150">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1595,24 +1745,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" customWidth="1"/>
-    <col min="5" max="5" width="29.88671875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" style="7" customWidth="1"/>
-    <col min="7" max="9" width="7.6640625" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="69.44140625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="7" customWidth="1"/>
+    <col min="7" max="9" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" style="7" customWidth="1"/>
+    <col min="11" max="11" width="67.85546875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="34.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" ht="34.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>16</v>
       </c>
@@ -1626,7 +1776,7 @@
       <c r="I1" s="16"/>
       <c r="J1" s="17"/>
     </row>
-    <row r="2" spans="1:23" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>18</v>
       </c>
@@ -1673,7 +1823,7 @@
       <c r="V2" s="15"/>
       <c r="W2" s="15"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>19</v>
       </c>
@@ -1706,7 +1856,7 @@
       </c>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>19</v>
       </c>
@@ -1739,7 +1889,7 @@
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>19</v>
       </c>
@@ -1772,7 +1922,7 @@
       </c>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>19</v>
       </c>
@@ -1805,7 +1955,7 @@
       </c>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>19</v>
       </c>
@@ -1840,7 +1990,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>19</v>
       </c>
@@ -1875,7 +2025,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
@@ -1910,7 +2060,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
@@ -1945,7 +2095,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>19</v>
       </c>
@@ -1980,7 +2130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>19</v>
       </c>
@@ -2015,7 +2165,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>19</v>
       </c>
@@ -2050,7 +2200,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>19</v>
       </c>
@@ -2085,7 +2235,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>19</v>
       </c>
@@ -2118,7 +2268,7 @@
       </c>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>19</v>
       </c>
@@ -2153,7 +2303,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>19</v>
       </c>
@@ -2188,7 +2338,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>19</v>
       </c>
@@ -2223,7 +2373,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>19</v>
       </c>
@@ -2258,7 +2408,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>19</v>
       </c>
@@ -2291,7 +2441,7 @@
       </c>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>19</v>
       </c>
@@ -2324,7 +2474,7 @@
       </c>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>19</v>
       </c>
@@ -2357,7 +2507,7 @@
       </c>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>50</v>
       </c>
@@ -2390,7 +2540,7 @@
       </c>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>50</v>
       </c>
@@ -2423,7 +2573,7 @@
       </c>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>50</v>
       </c>
@@ -2456,7 +2606,7 @@
       </c>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>50</v>
       </c>
@@ -2489,7 +2639,7 @@
       </c>
       <c r="K26" s="6"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>50</v>
       </c>
@@ -2522,7 +2672,7 @@
       </c>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>50</v>
       </c>
@@ -2555,7 +2705,7 @@
       </c>
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>50</v>
       </c>
@@ -2588,7 +2738,7 @@
       </c>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>50</v>
       </c>
@@ -2621,7 +2771,7 @@
       </c>
       <c r="K30" s="6"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>50</v>
       </c>
@@ -2654,538 +2804,538 @@
       </c>
       <c r="K31" s="6"/>
     </row>
-    <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="L2:W2"/>
     <mergeCell ref="A1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="F16:I16 F20:I20 G17:G18">
-    <cfRule type="containsText" dxfId="131" priority="167" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="149" priority="167" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="168" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="148" priority="168" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:I6 H7:I9">
-    <cfRule type="containsText" dxfId="129" priority="157" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="147" priority="157" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="128" priority="158" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="146" priority="158" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="containsText" dxfId="127" priority="161" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="145" priority="161" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="162" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="144" priority="162" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="containsText" dxfId="125" priority="159" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="143" priority="159" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",I3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="160" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="142" priority="160" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",I3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15:I15">
-    <cfRule type="containsText" dxfId="123" priority="155" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="141" priority="155" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="156" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="140" priority="156" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:G7 F10:I10 F8:F9">
-    <cfRule type="containsText" dxfId="121" priority="153" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="139" priority="153" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="154" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="138" priority="154" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:G13">
-    <cfRule type="containsText" dxfId="119" priority="151" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="137" priority="151" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="152" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="136" priority="152" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:I13">
-    <cfRule type="containsText" dxfId="117" priority="147" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="135" priority="147" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",I11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="148" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="134" priority="148" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",I11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="containsText" dxfId="115" priority="145" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="133" priority="145" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="146" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="132" priority="146" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="containsText" dxfId="113" priority="143" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="131" priority="143" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="144" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="130" priority="144" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="containsText" dxfId="111" priority="141" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="129" priority="141" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="142" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="128" priority="142" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="containsText" dxfId="109" priority="139" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="127" priority="139" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="140" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="126" priority="140" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:K3">
-    <cfRule type="containsText" dxfId="107" priority="137" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="125" priority="137" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="138" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="124" priority="138" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:K20">
-    <cfRule type="containsText" dxfId="105" priority="135" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="123" priority="135" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="136" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="122" priority="136" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:K15">
-    <cfRule type="containsText" dxfId="103" priority="119" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="121" priority="119" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="120" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="120" priority="120" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:K11 J12:J13">
-    <cfRule type="containsText" dxfId="101" priority="117" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="119" priority="117" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="118" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="118" priority="118" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:K7 K10 J8:J9">
-    <cfRule type="containsText" dxfId="99" priority="115" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="117" priority="115" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="116" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="116" priority="116" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:K6">
-    <cfRule type="containsText" dxfId="97" priority="113" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="115" priority="113" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="114" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="114" priority="114" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:K16 J17:J18">
-    <cfRule type="containsText" dxfId="95" priority="121" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="113" priority="121" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="122" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="112" priority="122" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="containsText" dxfId="93" priority="111" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="111" priority="111" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="112" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="110" priority="112" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14">
-    <cfRule type="containsText" dxfId="91" priority="109" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="109" priority="109" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="110" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="108" priority="110" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="containsText" dxfId="89" priority="107" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="107" priority="107" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",I14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="108" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="106" priority="108" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",I14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:K14">
-    <cfRule type="containsText" dxfId="87" priority="101" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="105" priority="101" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="102" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="104" priority="102" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:K19">
-    <cfRule type="containsText" dxfId="85" priority="97" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="103" priority="97" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="98" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="102" priority="98" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="containsText" dxfId="83" priority="105" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="101" priority="105" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="106" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="100" priority="106" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="containsText" dxfId="81" priority="103" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="99" priority="103" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="104" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="98" priority="104" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19:I19">
-    <cfRule type="containsText" dxfId="79" priority="99" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="97" priority="99" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="100" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="96" priority="100" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22:I22">
-    <cfRule type="containsText" dxfId="77" priority="95" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="95" priority="95" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="96" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="94" priority="96" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:K22">
-    <cfRule type="containsText" dxfId="75" priority="93" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="93" priority="93" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="94" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="92" priority="94" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:I4">
-    <cfRule type="containsText" dxfId="73" priority="91" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="91" priority="91" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="92" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="90" priority="92" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:K4">
-    <cfRule type="containsText" dxfId="71" priority="89" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="89" priority="89" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="90" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="88" priority="90" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G9">
-    <cfRule type="containsText" dxfId="69" priority="87" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="87" priority="87" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="88" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="86" priority="88" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="containsText" dxfId="67" priority="85" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="85" priority="85" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",K8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="86" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="84" priority="86" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",K8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="containsText" dxfId="65" priority="69" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="83" priority="69" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="70" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="82" priority="70" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="containsText" dxfId="63" priority="71" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="81" priority="71" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="72" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="80" priority="72" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="containsText" dxfId="61" priority="79" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="79" priority="79" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",K9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="80" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="78" priority="80" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",K9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="containsText" dxfId="59" priority="67" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="77" priority="67" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",K12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="68" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="76" priority="68" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",K12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="containsText" dxfId="57" priority="59" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="75" priority="59" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="60" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="74" priority="60" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="containsText" dxfId="55" priority="57" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="73" priority="57" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",K13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="58" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="72" priority="58" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",K13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="containsText" dxfId="53" priority="61" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="71" priority="61" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="62" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="70" priority="62" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18 H18:I18">
-    <cfRule type="containsText" dxfId="51" priority="55" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="69" priority="55" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="56" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="68" priority="56" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="containsText" dxfId="49" priority="53" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="67" priority="53" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",K18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="54" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="66" priority="54" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",K18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17">
-    <cfRule type="containsText" dxfId="47" priority="49" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="65" priority="49" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",K17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="50" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="64" priority="50" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",K17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17 H17:I17">
-    <cfRule type="containsText" dxfId="45" priority="51" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="63" priority="51" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="52" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="62" priority="52" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21:K21">
-    <cfRule type="containsText" dxfId="43" priority="45" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="61" priority="45" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="46" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="60" priority="46" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21:I21">
-    <cfRule type="containsText" dxfId="41" priority="47" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="59" priority="47" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="48" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="58" priority="48" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:I5">
-    <cfRule type="containsText" dxfId="39" priority="43" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="57" priority="43" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="44" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="56" priority="44" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:K5">
-    <cfRule type="containsText" dxfId="37" priority="41" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="55" priority="41" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="42" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="54" priority="42" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23:I23">
-    <cfRule type="containsText" dxfId="35" priority="39" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="53" priority="39" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="40" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="52" priority="40" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23:K23">
-    <cfRule type="containsText" dxfId="33" priority="37" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="51" priority="37" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="38" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="50" priority="38" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24:I24">
-    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="49" priority="35" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="48" priority="36" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:K24">
-    <cfRule type="containsText" dxfId="29" priority="33" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="47" priority="33" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="34" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="46" priority="34" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25:I25">
-    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="45" priority="31" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="44" priority="32" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25:K25">
-    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="43" priority="29" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="42" priority="30" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26:I26">
-    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="41" priority="23" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="40" priority="24" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26:K26">
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="39" priority="21" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="38" priority="22" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27:I27">
-    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="37" priority="19" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="36" priority="20" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J27:K27">
-    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="35" priority="17" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="34" priority="18" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:I28">
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="33" priority="15" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="32" priority="16" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28:K28">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="31" priority="13" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="30" priority="14" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29:I29">
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="29" priority="11" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="28" priority="12" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29:K29">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="27" priority="9" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="26" priority="10" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30:I30">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="25" priority="7" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="24" priority="8" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J30:K30">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31:I31">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31:K31">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J31)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3198,6 +3348,173 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="34.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="7"/>
+    </row>
+    <row r="2" spans="1:23" ht="66.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="L2:W2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="J3">
+    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",J3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",J3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",G3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",G3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",H3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",I3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",I3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Enter a valid CRUD function" error="Only &quot;Create&quot;, &quot;Read&quot;, &quot;Update&quot;, or &quot;Delete&quot; are allowed values. Please enter a valid value." sqref="F3:J3">
+      <formula1>"True, False"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>